<commit_message>
upload V2.1 files and Cmount adaptor 3D model
</commit_message>
<xml_diff>
--- a/Gerber/BOM_IMX294.xlsx
+++ b/Gerber/BOM_IMX294.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\will1\Dropbox\KiCad\IMX294_MIPI_Breakout_Small\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\will1\Dropbox\KiCad\FourThirdsEye_Small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E8F7C7-4C72-4331-BF53-51AD59B10C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD664D1-2E73-4831-BE53-CB09EA493DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3548" yWindow="1508" windowWidth="25829" windowHeight="15734" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="518" yWindow="1005" windowWidth="24682" windowHeight="13118" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
   <si>
     <t>Comment</t>
   </si>
@@ -234,21 +234,12 @@
     <t>C2049745</t>
   </si>
   <si>
-    <t>J5,J4,J3</t>
-  </si>
-  <si>
     <t>FL4,FL2,FL1,FL3,FL5</t>
   </si>
   <si>
     <t>R10,R3,R4,R8</t>
   </si>
   <si>
-    <t>C1,C36,C53,C4,C18,C6,C17,C43,C62,C24,C28,C38,C61,C52,C50,C47,C3,C8,C27,C34,C58,C29</t>
-  </si>
-  <si>
-    <t>C70,C41,C55,C45,C66,C46,C49,C31,C2,C22,C54,C59,C56,C65,C64,C9,C71,C33,C57,C16,C72,C63,C23</t>
-  </si>
-  <si>
     <t>C32,C37,C44,C21,C13,C35,C10,C25,C39,C26,C19,C48,C15</t>
   </si>
   <si>
@@ -258,9 +249,6 @@
     <t>R1,R2</t>
   </si>
   <si>
-    <t>C68,C67</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
@@ -297,9 +285,6 @@
     <t>JST_SH_BM04B-SRSS-TB_1x04-1MP_P1.00mm_Vertical</t>
   </si>
   <si>
-    <t>XF2M22151A</t>
-  </si>
-  <si>
     <t>NFM18CC101R1C3D</t>
   </si>
   <si>
@@ -349,6 +334,36 @@
   </si>
   <si>
     <t>C3211477</t>
+  </si>
+  <si>
+    <t>TF3822S05SV830</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>ICM-42688-P</t>
+  </si>
+  <si>
+    <t>PQFN50P300X250X97-14N</t>
+  </si>
+  <si>
+    <t>C1,C36,C53,C4,C18,C6,C17,C75,C43,C62,C24,C28,C38,C61,C52,C50,C47,C67,C3,C8,C27,C34,C58,C29</t>
+  </si>
+  <si>
+    <t>C68,C74</t>
+  </si>
+  <si>
+    <t>C70,C41,C55,C45,C66,C46,C49,C31,C2,C22,C54,C59,C73,C56,C65,C64,C9,C71,C33,C57,C16,C72,C63,C23</t>
+  </si>
+  <si>
+    <t>C1850418</t>
+  </si>
+  <si>
+    <t>C6552695</t>
+  </si>
+  <si>
+    <t>J4,J3</t>
   </si>
 </sst>
 </file>
@@ -448,7 +463,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -479,10 +494,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
@@ -833,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="20" customHeight="1"/>
@@ -864,26 +875,26 @@
         <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>51</v>
@@ -896,7 +907,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>9</v>
@@ -912,7 +923,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>9</v>
@@ -925,32 +936,32 @@
     </row>
     <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -960,7 +971,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>7</v>
@@ -976,12 +987,12 @@
         <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="7" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="6"/>
@@ -992,13 +1003,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -1008,12 +1019,12 @@
         <v>55</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>56</v>
       </c>
       <c r="E11" s="6"/>
@@ -1024,7 +1035,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>10</v>
@@ -1037,32 +1048,32 @@
     </row>
     <row r="13" spans="1:6" ht="20" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" ht="20" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1072,7 +1083,7 @@
         <v>45</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>25</v>
@@ -1085,15 +1096,17 @@
     </row>
     <row r="16" spans="1:6" ht="20" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="6"/>
+        <v>93</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
@@ -1114,16 +1127,16 @@
     </row>
     <row r="18" spans="1:6" ht="20" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1133,29 +1146,29 @@
         <v>12</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="20" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -1181,7 +1194,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>6</v>
@@ -1225,11 +1238,11 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="20" customHeight="1">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>43</v>
@@ -1289,10 +1302,18 @@
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" ht="20" customHeight="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+      <c r="A29" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
       <c r="A34" s="6"/>

</xml_diff>